<commit_message>
Cleaned up formatting on Parts List
</commit_message>
<xml_diff>
--- a/Parts List.xlsx
+++ b/Parts List.xlsx
@@ -137,16 +137,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -171,18 +171,19 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -498,11 +499,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -511,97 +510,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>1</v>
       </c>
+      <c r="C9" s="2"/>
       <c r="D9" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>2</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -609,13 +628,13 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>1</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -623,38 +642,56 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="5"/>
       <c r="D13" s="4"/>
     </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>1</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>1</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>